<commit_message>
upload files for iteration one by xiang
</commit_message>
<xml_diff>
--- a/Document/CS673F16Team3_weeklyreport.xlsx
+++ b/Document/CS673F16Team3_weeklyreport.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="81">
   <si>
     <t>week #
  (from date - end date)</t>
@@ -72,6 +72,9 @@
     <t>04/09 - 11/09</t>
   </si>
   <si>
+    <t>making plan</t>
+  </si>
+  <si>
     <t xml:space="preserve">discuss initial plan </t>
   </si>
   <si>
@@ -90,6 +93,9 @@
     <t>20/09 - 26/09</t>
   </si>
   <si>
+    <t>Yansen Liu</t>
+  </si>
+  <si>
     <t>discuss initial plan; 
 set up configuration; 
 teach team members about using git and github;
@@ -102,16 +108,65 @@
     <t>1,2,3,5</t>
   </si>
   <si>
+    <t>design requirements in SPPP, design app</t>
+  </si>
+  <si>
+    <t>27/09-04/10</t>
+  </si>
+  <si>
+    <t>register domain name;
+set up web site host;
+deploy our website on the host;
+code review;
+pair programming;
+handle github pull request;
+wirte weekly meeting report;
+discuss about the front-end web design;
+create user story on the pivottracker;</t>
+  </si>
+  <si>
+    <t>0,1,2,4</t>
+  </si>
+  <si>
+    <t>xiang chen</t>
+  </si>
+  <si>
+    <t>05/10 - 18/10</t>
+  </si>
+  <si>
+    <t>create issue on github;
+make code change about the front-end;
+create sql file and upload to github;
+write user story on the pivot tracker;
+learning php language
+solve domain issue</t>
+  </si>
+  <si>
+    <t>1,2,3,4</t>
+  </si>
+  <si>
+    <t>UI design, practice presentation, SPPP, logo design</t>
+  </si>
+  <si>
+    <t>UI design, set MAMP environment</t>
+  </si>
+  <si>
     <t>0,1,2 ,5, 6 Writing SPPP Draft; 
 Learning PHP and SQL security; 
 Discusing requirements and features</t>
   </si>
   <si>
-    <t>making plan</t>
+    <t>05/10-11/10</t>
   </si>
   <si>
     <t>SPPP Final Draft;
 Presentation;</t>
+  </si>
+  <si>
+    <t>UI design, front-end review and coding, user story design</t>
+  </si>
+  <si>
+    <t>12/10-18/10</t>
   </si>
   <si>
     <t xml:space="preserve">0, 1, 2, 5, 6 Finalizing SPPP;
@@ -125,13 +180,61 @@
 Security Document;</t>
   </si>
   <si>
-    <t>Yansen Liu</t>
+    <t>prepare for presentation 2, front-end inplementation</t>
   </si>
   <si>
-    <t>design requirements in SPPP, design app</t>
+    <t>27/09 - 04/10</t>
   </si>
   <si>
-    <t>UI design, practice presentation, SPPP, logo design</t>
+    <t xml:space="preserve">0, 2, 5, 6 Writing Security Document;
+Learning php back end security issue;
+Discussion with Yansen about UI design;
+</t>
+  </si>
+  <si>
+    <t>Implement prototype for interation 1;</t>
+  </si>
+  <si>
+    <t>05/10 - 11/10</t>
+  </si>
+  <si>
+    <t>0, 1, 2, 3, 5, 6
+Assist Yansen about three parts of UI we need for Sprint 1;
+Learn JQuery and PHP for finishing three User Stories;
+Choose three User Stories as Sprint 1 objective;</t>
+  </si>
+  <si>
+    <t>Prepare PPT for presentation;
+Finish up implementation for Sprint 1;
+Host weekly meeting when Dawei is not available</t>
+  </si>
+  <si>
+    <t>12/10 - 18/10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0, 3, 5, 6
+Prepare PPT for presentation;
+Assist Yansen with UI finalization;
+</t>
+  </si>
+  <si>
+    <t>Requirement Anaylze for Sprint 2;
+Refactor good and bad for Sprint 1;
+Implementation for Spring 2;
+Securtiy Learning;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,1,2,5 Gathered for first meeting, discuss the overview
+of our product.Allocating roles and tasks. Learning about
+enviroment configuration.
+</t>
+  </si>
+  <si>
+    <t>0,1,2,5</t>
+  </si>
+  <si>
+    <t>0,1,2,5 Discuss requirements, designing interface, asking
+questions about confusing part in order to settle for inplementation</t>
   </si>
   <si>
     <t xml:space="preserve">0, gathered the tutorial for learning html, CSS, JQuery
@@ -140,6 +243,23 @@
      come up with the project name "return to_powerof_a", and the team name"Hello_world"
 5, set up slack channel and github repository. Come up with a github practice that ensures every team member is able to update the code
     Github practice: update the README.md file with everyone's name and role </t>
+  </si>
+  <si>
+    <t>0,1,2,3,5</t>
+  </si>
+  <si>
+    <t>1,2,5,6 Preparing presentation, task breakdown for implementation,</t>
+  </si>
+  <si>
+    <t>0,1,2,3,4,5</t>
+  </si>
+  <si>
+    <t>27/09 - 4/10</t>
+  </si>
+  <si>
+    <t>0,1,2,3,5 Learning about PHP myadmin, discussing requirements,
+communicating programming skills, implement some of the simple
+code and SQL sentences.</t>
   </si>
   <si>
     <t>11/09 - 18/09</t>
@@ -160,26 +280,22 @@
 6, do the presentation</t>
   </si>
   <si>
-    <t xml:space="preserve">0,1,2,5 Gathered for first meeting, discuss the overview
-of our product.Allocating roles and tasks. Learning about
-enviroment configuration.
+    <t xml:space="preserve">0,learned how to use MAMP to set up local host and do the test, learned PHP, HTML5, CSS, javascript
+1, come up with an aproach to realize the main function we need(how to asign backlogs to each sprint)
 </t>
   </si>
   <si>
-    <t>0,1,2,5</t>
+    <t>1, created user stories and calculate its points 
+    draw class diagram and make plan of our project develpment
+3, help Weicheng to build the UI by using HTML, CSS
+    connect MySQL with PHP
+4, look for PHP unit test module
+5, assign works to team members</t>
   </si>
   <si>
-    <t>0,1,2,5 Discuss requirements, designing interface, asking
-questions about confusing part in order to settle for inplementation</t>
-  </si>
-  <si>
-    <t>0,1,2,3,5</t>
-  </si>
-  <si>
-    <t>1,2,5,6 Preparing presentation, task breakdown for implementation,</t>
-  </si>
-  <si>
-    <t>0,1,2,3,4,5</t>
+    <t xml:space="preserve">3, programming frontend HTML and backend PHP
+5,    coordinate team members work flow and plan the development in the big picture
+</t>
   </si>
   <si>
     <t>0,1,5,6
@@ -195,6 +311,28 @@
 learn to use testing tools.</t>
   </si>
   <si>
+    <t>0,1,3,5
+learn php,
+learn how to use MAMP to test,
+programming,
+discuss and improve features</t>
+  </si>
+  <si>
+    <t>0,1,4,5
+learn php,
+unit testing,
+programming,
+discuss and get feedback from 
+invited users</t>
+  </si>
+  <si>
+    <t>0,1,4,5
+write test code,
+prepare interation one presentation,
+discuss presentation details,
+compatibility testing</t>
+  </si>
+  <si>
     <t>0 - learning the product metrics and process metrics,1 - requirement analysis analyze how the quality metrics should involve and how can every design leader get involved ,2 - design for quality assurance steps and process</t>
   </si>
   <si>
@@ -205,6 +343,23 @@
   </si>
   <si>
     <t>UML diagram finish and database creation</t>
+  </si>
+  <si>
+    <t>0,1,2,3,5 Learning about PHP myadmin, discussing requirements,
+communicating programming skills, review and change database diagram and creatre new attributes</t>
+  </si>
+  <si>
+    <t>0,2,4,5</t>
+  </si>
+  <si>
+    <t>05/10 - 15/10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+revise databse design
+write user story on the pivot tracker;
+learning php language
+solve domain issue</t>
   </si>
 </sst>
 </file>
@@ -222,14 +377,14 @@
     </font>
     <font/>
     <font>
-      <color rgb="FFFF0000"/>
-    </font>
-    <font>
       <color rgb="FF000000"/>
     </font>
     <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <color rgb="FFFF0000"/>
     </font>
   </fonts>
   <fills count="3">
@@ -252,38 +407,41 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" vertical="bottom"/>
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
+      <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -298,7 +456,6 @@
           <bgColor rgb="FFB7E1CD"/>
         </patternFill>
       </fill>
-      <alignment/>
       <border/>
     </dxf>
   </dxfs>
@@ -335,9 +492,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -424,7 +578,7 @@
         <v>2.0</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F2" s="3">
         <v>2.0</v>
@@ -438,7 +592,7 @@
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N2" s="3">
         <v>10.0</v>
@@ -446,7 +600,7 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
@@ -459,7 +613,7 @@
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" s="3">
         <v>10.0</v>
@@ -471,7 +625,7 @@
         <v>4.0</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F3" s="3">
         <v>2.0</v>
@@ -489,12 +643,12 @@
         <v>10.0</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" ht="78.75" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" s="3">
         <v>10.0</v>
@@ -506,7 +660,7 @@
         <v>2.0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3">
         <v>1.0</v>
@@ -528,7 +682,7 @@
         <v>1.0</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="N4" s="3">
         <v>10.0</v>
@@ -536,7 +690,7 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
@@ -548,22 +702,53 @@
       <c r="Y4" s="2"/>
     </row>
     <row r="5" ht="49.5" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="3">
+        <v>12.0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>10.0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="H5" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="J5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="K5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="L5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" s="3">
+        <v>10.0</v>
+      </c>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
+      <c r="Q5" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
@@ -574,18 +759,48 @@
       <c r="Y5" s="2"/>
     </row>
     <row r="6" ht="34.5" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="3">
+        <v>10.0</v>
+      </c>
+      <c r="C6" s="3">
+        <v>8.0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="H6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="J6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="K6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="L6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6" s="3">
+        <v>10.0</v>
+      </c>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
@@ -784,7 +999,7 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
-      <c r="L14" s="5"/>
+      <c r="L14" s="7"/>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
       <c r="O14" s="2"/>
@@ -896,7 +1111,7 @@
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
-      <c r="L20" s="5"/>
+      <c r="L20" s="7"/>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
       <c r="O20" s="2"/>
@@ -1008,7 +1223,7 @@
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
-      <c r="L26" s="5"/>
+      <c r="L26" s="7"/>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
       <c r="O26" s="2"/>
@@ -1120,7 +1335,7 @@
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
-      <c r="L32" s="5"/>
+      <c r="L32" s="7"/>
       <c r="M32" s="3"/>
       <c r="N32" s="3"/>
       <c r="O32" s="2"/>
@@ -1232,7 +1447,7 @@
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
-      <c r="L38" s="5"/>
+      <c r="L38" s="7"/>
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
       <c r="O38" s="2"/>
@@ -1344,7 +1559,7 @@
       <c r="I44" s="3"/>
       <c r="J44" s="3"/>
       <c r="K44" s="3"/>
-      <c r="L44" s="5"/>
+      <c r="L44" s="7"/>
       <c r="M44" s="3"/>
       <c r="N44" s="3"/>
       <c r="O44" s="2"/>
@@ -1456,7 +1671,7 @@
       <c r="I50" s="3"/>
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
-      <c r="L50" s="5"/>
+      <c r="L50" s="7"/>
       <c r="M50" s="3"/>
       <c r="N50" s="3"/>
       <c r="O50" s="2"/>
@@ -1568,7 +1783,7 @@
       <c r="I56" s="3"/>
       <c r="J56" s="3"/>
       <c r="K56" s="3"/>
-      <c r="L56" s="5"/>
+      <c r="L56" s="7"/>
       <c r="M56" s="3"/>
       <c r="N56" s="3"/>
       <c r="O56" s="2"/>
@@ -13844,15 +14059,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="5" max="5" width="47.71"/>
+    <col customWidth="1" min="13" max="13" width="37.29"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -13916,7 +14129,7 @@
         <v>4.0</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F2" s="3">
         <v>1.0</v>
@@ -13949,7 +14162,7 @@
     </row>
     <row r="3" ht="36.75" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" s="3">
         <v>6.0</v>
@@ -13961,7 +14174,7 @@
         <v>2.0</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="F3" s="3">
         <v>2.0</v>
@@ -13985,7 +14198,7 @@
         <v>0.0</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="N3" s="3">
         <v>10.0</v>
@@ -13993,7 +14206,7 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" s="3">
         <v>8.0</v>
@@ -14005,7 +14218,7 @@
         <v>2.0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="F4" s="3">
         <v>2.0</v>
@@ -14029,9 +14242,141 @@
         <v>1.0</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="N4" s="3">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="3">
+        <v>8.0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="K5" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="L5" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="N5" s="3">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="3">
+        <v>8.0</v>
+      </c>
+      <c r="C6" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="H6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I6" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="K6" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="L6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="N6" s="3">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="3">
+        <v>10.0</v>
+      </c>
+      <c r="C7" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="K7" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="L7" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="N7" s="3">
         <v>10.0</v>
       </c>
     </row>
@@ -14042,9 +14387,6 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -14122,7 +14464,7 @@
         <v>4.0</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="F2" s="3">
         <v>2.0</v>
@@ -14142,7 +14484,7 @@
       <c r="K2" s="3">
         <v>1.0</v>
       </c>
-      <c r="L2" s="6">
+      <c r="L2" s="5">
         <v>0.0</v>
       </c>
       <c r="M2" s="3">
@@ -14150,12 +14492,12 @@
       </c>
       <c r="N2" s="3"/>
       <c r="P2" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" s="3">
         <v>9.0</v>
@@ -14167,7 +14509,7 @@
         <v>4.0</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F3" s="3">
         <v>1.0</v>
@@ -14190,10 +14532,13 @@
       <c r="L3" s="3">
         <v>0.0</v>
       </c>
+      <c r="M3" s="3">
+        <v>6.0</v>
+      </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="7" t="s">
-        <v>20</v>
+      <c r="A4" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="B4" s="3">
         <v>7.0</v>
@@ -14205,7 +14550,7 @@
         <v>2.0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F4" s="3">
         <v>1.0</v>
@@ -14230,6 +14575,123 @@
       </c>
       <c r="M4" s="3">
         <v>6.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="K5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="L5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M5" s="3">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="3">
+        <v>9.0</v>
+      </c>
+      <c r="C6" s="3">
+        <v>7.0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="H6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I6" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="K6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="L6" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="3">
+        <v>10.0</v>
+      </c>
+      <c r="C7" s="3">
+        <v>8.0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="H7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="K7" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="L7" s="3">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>
@@ -14244,11 +14706,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
@@ -14268,7 +14730,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -14323,8 +14785,8 @@
       <c r="D2" s="3">
         <v>4.0</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>31</v>
+      <c r="E2" s="9" t="s">
+        <v>55</v>
       </c>
       <c r="F2" s="3">
         <v>2.0</v>
@@ -14344,7 +14806,7 @@
       <c r="K2" s="3">
         <v>1.0</v>
       </c>
-      <c r="L2" s="9">
+      <c r="L2" s="10">
         <v>0.0</v>
       </c>
       <c r="M2" s="3">
@@ -14365,7 +14827,7 @@
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="B3" s="3">
         <v>14.0</v>
@@ -14376,8 +14838,8 @@
       <c r="D3" s="3">
         <v>4.0</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>33</v>
+      <c r="E3" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="F3" s="3">
         <v>5.0</v>
@@ -14407,7 +14869,7 @@
     </row>
     <row r="4" ht="59.25" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="B4" s="3">
         <v>8.0</v>
@@ -14418,8 +14880,8 @@
       <c r="D4" s="3">
         <v>2.0</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>35</v>
+      <c r="E4" s="11" t="s">
+        <v>64</v>
       </c>
       <c r="F4" s="3">
         <v>1.0</v>
@@ -14444,6 +14906,100 @@
       </c>
       <c r="M4" s="3">
         <v>0.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="3">
+        <v>8.0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="L5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="N5" s="3"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="3">
+        <v>8.0</v>
+      </c>
+      <c r="C6" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="J6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="K6" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="3">
+        <v>10.0</v>
+      </c>
+      <c r="C7" s="3">
+        <v>7.0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="I7" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="K7" s="3">
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>
@@ -14458,15 +15014,12 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="5" max="5" width="54.86"/>
+    <col customWidth="1" min="5" max="5" width="56.86"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -14527,7 +15080,7 @@
         <v>4.0</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="F2" s="3">
         <v>2.0</v>
@@ -14547,11 +15100,11 @@
       <c r="K2" s="3">
         <v>1.0</v>
       </c>
-      <c r="L2" s="6">
+      <c r="L2" s="5">
         <v>0.0</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="N2" s="3">
         <v>8.0</v>
@@ -14560,7 +15113,7 @@
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" s="3">
         <v>6.0</v>
@@ -14572,7 +15125,7 @@
         <v>4.0</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="F3" s="3">
         <v>0.5</v>
@@ -14596,15 +15149,15 @@
         <v>0.0</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="N3" s="3">
-        <v>12.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="7" t="s">
-        <v>20</v>
+      <c r="A4" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="B4" s="3">
         <v>5.0</v>
@@ -14616,7 +15169,7 @@
         <v>2.0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="F4" s="3">
         <v>1.0</v>
@@ -14640,9 +15193,53 @@
         <v>0.0</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="N4" s="3">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="K5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="L5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="N5" s="3">
         <v>10.0</v>
       </c>
     </row>
@@ -14658,9 +15255,6 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -14726,7 +15320,7 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" s="3">
         <v>10.0</v>
@@ -14738,7 +15332,7 @@
         <v>4.0</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="F2" s="3">
         <v>3.0</v>
@@ -14756,7 +15350,7 @@
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3" s="3">
         <v>6.0</v>
@@ -14768,7 +15362,7 @@
         <v>2.0</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="F3" s="3">
         <v>2.0</v>
@@ -14777,6 +15371,93 @@
         <v>1.0</v>
       </c>
       <c r="K3" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="3">
+        <v>7.0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="K4" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="3">
+        <v>10.0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>8.0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="J5" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="K5" s="3">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="3">
+        <v>13.0</v>
+      </c>
+      <c r="C6" s="3">
+        <v>9.0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="J6" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="K6" s="3">
         <v>1.0</v>
       </c>
     </row>
@@ -14787,9 +15468,6 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -14860,7 +15538,7 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" s="3">
         <v>9.0</v>
@@ -14871,8 +15549,8 @@
       <c r="D2" s="3">
         <v>4.0</v>
       </c>
-      <c r="E2" s="10" t="s">
-        <v>44</v>
+      <c r="E2" s="11" t="s">
+        <v>73</v>
       </c>
       <c r="F2" s="3">
         <v>1.0</v>
@@ -14896,12 +15574,12 @@
         <v>0.0</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3" s="3">
         <v>8.0</v>
@@ -14912,8 +15590,8 @@
       <c r="D3" s="3">
         <v>2.0</v>
       </c>
-      <c r="E3" s="11" t="s">
-        <v>46</v>
+      <c r="E3" s="12" t="s">
+        <v>75</v>
       </c>
       <c r="F3" s="3">
         <v>2.0</v>
@@ -14937,11 +15615,110 @@
         <v>1.0</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="N3" s="3">
         <v>10.0</v>
       </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="H4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="J4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="L4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="N4" s="3">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="5" ht="34.5" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="3">
+        <v>10.0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="J5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="K5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="L5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="N5" s="3">
+        <v>10.0</v>
+      </c>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>